<commit_message>
aktualizacja odnośnie zarysu gry
</commit_message>
<xml_diff>
--- a/_game/zarys gry.xlsx
+++ b/_game/zarys gry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24911"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BBDB1A-4EE8-4BC4-AFAD-23A7DD56E0E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E66EBE52-7126-4881-9604-36C157ACDF33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,23 @@
     <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>seba</t>
   </si>
@@ -30,64 +41,148 @@
     <t>pjoter</t>
   </si>
   <si>
+    <t xml:space="preserve">pomysły pewne, akceptujemy </t>
+  </si>
+  <si>
+    <t>technikalia/ progamowanie</t>
+  </si>
+  <si>
     <t>Typ gry</t>
   </si>
   <si>
+    <t xml:space="preserve">H&amp;S z dungeonami, raczej </t>
+  </si>
+  <si>
+    <t>open word generowany proceduralnie. Klimat sztywny, czy bimber wspomaga siłę, leczysz się piwem, na wampiry idziesz z sosem czosnkowym na zębach, a manna potiony to jakiś niedziałający szajs który wymyśliły jakieś debile. Dodałbym fizykę. Podstawową, ale żeby była</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open World generowany proceduralnie. </t>
+  </si>
+  <si>
+    <t>Kamerę biorę na klatę. Pytanie, jak rozwiązać zejście do podziemi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zejścia do podziemi najlepiej zrobić na osobnej mapie. </t>
+  </si>
+  <si>
+    <t>klimat</t>
+  </si>
+  <si>
+    <t>Fantasy bądź może SF? Raczej stawiam na fantasy. Fabuła też do obgadania.</t>
+  </si>
+  <si>
+    <t>fantasy &lt;3 walić kosmos. Fabuła zarys - pretekst do open worda</t>
+  </si>
+  <si>
+    <t>fantasy</t>
+  </si>
+  <si>
+    <t>jaki styl graficzny pikseloza i kwadraty? W więcej bym nie szedł bo nie jestem lotny z grafiki</t>
+  </si>
+  <si>
+    <t>pikseloza i kwadraty</t>
+  </si>
+  <si>
+    <t>system postaci</t>
+  </si>
+  <si>
+    <t>Do dyskusji czy idziemy w jedną rasę (np. human) czy mamy kilka do wyboru. Klasy postaci na początek war i sorc</t>
+  </si>
+  <si>
+    <t>dałbym same krasnoludy. Pasują do robienia dungeonów. Symulator życia krasnoluda?</t>
+  </si>
+  <si>
+    <t>Symulator życia krasnoluda xD ale to tylko warek wtedy, lub hunter z gunem. Nie widzę krasnala jako maga w sukince</t>
+  </si>
+  <si>
+    <t>no tutaj IKSDE bo trzeba wiedzieć co programować</t>
+  </si>
+  <si>
+    <t>Sorc będzie miał dwie zmienne odnawialne (health i mana). nie wiem czy dla wara robić to samo, mana dla wara mi nie pasuje. Albo będzie miał tylko helth odnawialne a na spelle cooldown lub dodać mu zamiast many np. rage samo odnawialny</t>
+  </si>
+  <si>
+    <t>magia jest dla elfich gejów. Levelowanie jakieś tak, ale bez pierdololo w miliony statystyk. W sensie bez analizowania co do 0,0001% szansy na krytyka. Wolałbym rozwiazać to tak - przykład: idziesz na żywiołaka ognia -&gt; przygotowujesz eq wodne. Ale jak trafisz na lodowego, to Cię rozwala na drobne, bo lod zamraża wodę. Więc na lody idzie się z eq ognia, ale wtedy masakruje Cię woda... bo nic tak nie boli jak endgame, że jesteś przekozak.</t>
+  </si>
+  <si>
+    <t>Problem ze zbieraniem eq. Dojedzie do tego ze będziesz musiał zbierac co chwila inne eq. Albo dodać możliwość ulepszania odporności na dane żywioły. Chciałbym aby na konkretnego bosa była jakaś taktyka a nie tylko napierdalanie, wtedy możesz mieć zajebiste eq a i tak bosa nie ubijesz.</t>
+  </si>
+  <si>
+    <t>levelowanie, lvl cap czy no limit?</t>
+  </si>
+  <si>
+    <t>drzewko talentów?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">za każdy lvl punkty do rozdania do statystyk postaci (helth , str, int, dex) i drzewko talentów </t>
+  </si>
+  <si>
+    <t>EQ bym rozbudował. Ale tak bym to zrobił, żeby nie było wątpliwości co jest lepsze. W sensie nie musisz studiować każdego parametru - to ma wyjść instynktownie.</t>
+  </si>
+  <si>
+    <t>eq: bronie, pancerz, amulety, naszyjniki etc. Wymyślenie nazw i statystyk broni i pancerzy</t>
+  </si>
+  <si>
+    <t>Czyli prosto. Im więcej armowu tym lepiej. Broń im większy dmg tym lepiej?</t>
+  </si>
+  <si>
+    <t>Miejsce w plecaku mocno ograniczone</t>
+  </si>
+  <si>
+    <t>tak, zobacz na eq z x-com i podobnych. Jednocześnie nie wracasz z toną szpeju z wyprawy, a idziesz konkretnie po coś.</t>
+  </si>
+  <si>
+    <t>Tylko jeżeli chcemy robić mocny crafting to będzie problem z bagiem</t>
+  </si>
+  <si>
     <t>Crafting</t>
   </si>
   <si>
-    <t>klimat</t>
-  </si>
-  <si>
-    <t>Fantasy bądź może SF? Raczej stawiam na fantasy. Fabuła też do obgadania.</t>
-  </si>
-  <si>
-    <t>system postaci</t>
-  </si>
-  <si>
-    <t>Do dyskusji czy idziemy w jedną rasę (np. human) czy mamy kilka do wyboru. Klasy postaci na początek war i sorc</t>
-  </si>
-  <si>
-    <t>drzewko talentów?</t>
-  </si>
-  <si>
-    <t>Sorc będzie miał dwie zmienne odnawialne (health i mana). nie wiem czy dla wara robić to samo, mana dla wara mi nie pasuje. Albo będzie miał tylko helth odnawialne a na spelle cooldown lub dodać mu zamiast many np. rage samo odnawialny</t>
-  </si>
-  <si>
-    <t>levelowanie, lvl cap czy no limit?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">za każdy lvl punkty do rozdania do statystyk postaci (helth , str, int, dex) i drzewko talentów </t>
-  </si>
-  <si>
-    <t>eq: bronie, pancerz, amulety, naszyjniki etc. Wymyślenie nazw i statystyk broni i pancerzy</t>
+    <t>Tylko ulepszanie eq</t>
+  </si>
+  <si>
+    <t>full crafting każdego elementu gry. Ale bez zbierania 2134546 bryłek rudy, żeby wykłuć sztabę których 23142 potrzebujesz na sztylet</t>
+  </si>
+  <si>
+    <t>Wymyśleć system craftingu</t>
+  </si>
+  <si>
+    <t>trzeba zrobić item nr jeden. Potem to podmiana modelu i statystyka</t>
   </si>
   <si>
     <t>sterowanie</t>
   </si>
   <si>
+    <t>Widzę dwie sensowne opcje:</t>
+  </si>
+  <si>
+    <t>to samo. WSAD opanowałem, click and move starałem się ogarnąć. WSAD "upośledza" sterowanie, więc może to być zabawniejsze. Może wsad + action key?</t>
+  </si>
+  <si>
+    <t>moim zdaniem ze smamy wsadem będzie ciężko, można spróbować ale bez obsugi muszki wydaje mi sie ze nie damy rady. Może sam upośledzony wsad da urokowi grze. Do przetesowania</t>
+  </si>
+  <si>
+    <t>w sumie zaimplementowany jest wsad c&amp;m nie robiłem, ale powinno w miarę się ogarnąć sprawnie</t>
+  </si>
+  <si>
+    <t>1) wsad poruszamy postacią a kursor myszy pokazuje w którą stronę patrzymy.</t>
+  </si>
+  <si>
     <t>2) click and move czy coś ala z diablo.</t>
   </si>
   <si>
-    <t>Widzę dwie sensowne opcje:</t>
-  </si>
-  <si>
-    <t>1) wsad poruszamy postacią a kursor myszy pokazuje w którą stronę patrzymy.</t>
-  </si>
-  <si>
     <t>Mapa / świat</t>
   </si>
   <si>
     <t>Trzeba coś wygenerować xD ogólnie widzę to tak, że zaczynamy w miasteczku/wiosce czyli miejscu startowym. Można wyjść poza startówkę i nawalać się z mobami, robić questy. W zależności od rozwoju fabuły przechodzimy do nowych lokacjie.</t>
   </si>
   <si>
-    <t xml:space="preserve">H&amp;S z dungeonami, raczej </t>
-  </si>
-  <si>
-    <t>Miejsce w plecaku mocno ograniczone</t>
-  </si>
-  <si>
-    <t>Tylko ulepszanie eq</t>
+    <t xml:space="preserve">generujemy poki co płaską planszę. Do opanowania wq mnie jest to - 1 blok - 1lvl dungeonów?, czy generowanie coś jak minecraft i wielopoziomowe jaskinie - dungeony. Chce Ci się wymyślać questy? xD Wg mnie przy założeniu, że jesteśmy krasnoludami dać coś w stylu - jako pełnoletni, młody pełen wigoru 200 letni krasnolud, twój klan daje ci na wynos pota - bimber, podstawowe eq, zbydował ci u podnórza góry jakąś pipidówę i kazał założyć se swoj klan herby axa i hoocha </t>
+  </si>
+  <si>
+    <t>Nie wiem czy czasami wielopoziom nas nie przerośnie, ja bynajmniej nie mam na to pomysłu. Więc stawiam na razie na płaską planszę. Co do generowania znaleźć/wymyśleć algorytm i elo</t>
+  </si>
+  <si>
+    <t>generator… tu trzeba rozpisać jakieś algorytmy sensowne i sposób generowania / zapisu dancyh itp... W tym temacie to jesteśmy w dupie. A bawić się w level desinera nie chce - lepiej generator dać</t>
   </si>
   <si>
     <t>Potwory</t>
@@ -96,64 +191,19 @@
     <t>Wymyślenie przeciwników, z danego moba może wylecieć jakiś przedmiot. Bossy z lepszym eq</t>
   </si>
   <si>
-    <t>dałbym same krasnoludy. Pasują do robienia dungeonów. Symulator życia krasnoluda?</t>
-  </si>
-  <si>
-    <t>magia jest dla elfich gejów. Levelowanie jakieś tak, ale bez pierdololo w miliony statystyk. W sensie bez analizowania co do 0,0001% szansy na krytyka. Wolałbym rozwiazać to tak - przykład: idziesz na żywiołaka ognia -&gt; przygotowujesz eq wodne. Ale jak trafisz na lodowego, to Cię rozwala na drobne, bo lod zamraża wodę. Więc na lody idzie się z eq ognia, ale wtedy masakruje Cię woda... bo nic tak nie boli jak endgame, że jesteś przekozak.</t>
-  </si>
-  <si>
-    <t>EQ bym rozbudował. Ale tak bym to zrobił, żeby nie było wątpliwości co jest lepsze. W sensie nie musisz studiować każdego parametru - to ma wyjść instynktownie.</t>
-  </si>
-  <si>
-    <t>tak, zobacz na eq z x-com i podobnych. Jednocześnie nie wracasz z toną szpeju z wyprawy, a idziesz konkretnie po coś.</t>
-  </si>
-  <si>
-    <t>full crafting każdego elementu gry. Ale bez zbierania 2134546 bryłek rudy, żeby wykłuć sztabę których 23142 potrzebujesz na sztylet</t>
-  </si>
-  <si>
-    <t>to samo. WSAD opanowałem, click and move starałem się ogarnąć. WSAD "upośledza" sterowanie, więc może to być zabawniejsze. Może wsad + action key?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pomysły pewne, akceptujemy </t>
-  </si>
-  <si>
-    <t>fantasy &lt;3 walić kosmos. Fabuła zarys - pretekst do open worda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">generujemy poki co płaską planszę. Do opanowania wq mnie jest to - 1 blok - 1lvl dungeonów?, czy generowanie coś jak minecraft i wielopoziomowe jaskinie - dungeony. Chce Ci się wymyślać questy? xD Wg mnie przy założeniu, że jesteśmy krasnoludami dać coś w stylu - jako pełnoletni, młody pełen wigoru 200 letni krasnolud, twój klan daje ci na wynos pota - bimber, podstawowe eq, zbydował ci u podnórza góry jakąś pipidówę i kazał założyć se swoj klan herby axa i hoocha </t>
-  </si>
-  <si>
     <t>wolałbym, żeby z zapchlonej myszy nie wylatywał dwuręczny topór olbrzyma waligóry. Bossy tak. Pytanie w jaki kierunek idziemy.</t>
   </si>
   <si>
-    <t>technikalia/ progamowanie</t>
-  </si>
-  <si>
-    <t>open word generowany proceduralnie. Klimat sztywny, czy bimber wspomaga siłę, leczysz się piwem, na wampiry idziesz z sosem czosnkowym na zębach, a manna potiony to jakiś niedziałający szajs który wymyśliły jakieś debile. Dodałbym fizykę. Podstawową, ale żeby była</t>
-  </si>
-  <si>
-    <t>Kamerę biorę na klatę. Pytanie, jak rozwiązać zejście do podziemi.</t>
-  </si>
-  <si>
-    <t>jaki styl graficzny pikseloza i kwadraty? W więcej bym nie szedł bo nie jestem lotny z grafiki</t>
-  </si>
-  <si>
-    <t>no tutaj IKSDE bo trzeba wiedzieć co programować</t>
-  </si>
-  <si>
-    <t>trzeba zrobić item nr jeden. Potem to podmiana modelu i statystyka</t>
-  </si>
-  <si>
-    <t>w sumie zaimplementowany jest wsad c&amp;m nie robiłem, ale powinno w miarę się ogarnąć sprawnie</t>
-  </si>
-  <si>
-    <t>generator… tu trzeba rozpisać jakieś algorytmy sensowne i sposób generowania / zapisu dancyh itp... W tym temacie to jesteśmy w dupie. A bawić się w level desinera nie chce - lepiej generator dać</t>
+    <t>Z mobów wylatują itemy eq "zwykłe"  + itemy do craftingu. Z bosów lepsze itemy epiczne xD np. "złoty kufel pełny bimbru, kiedy kufel jest aktywny w eq to twoja szansa na trafienie spada o 50% ale dmg wzrasta o 50% xD"</t>
   </si>
   <si>
     <t>trza zaprogramować xD</t>
   </si>
   <si>
     <t>MULTIPLEJR….</t>
+  </si>
+  <si>
+    <t>W  dalekiej przyszłości...</t>
   </si>
 </sst>
 </file>
@@ -193,7 +243,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,6 +269,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6E0B4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFB5D3"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -267,7 +329,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -281,19 +343,28 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -305,6 +376,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFB5D3"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -317,9 +393,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -357,7 +433,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -463,7 +539,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -637,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -649,14 +725,14 @@
     <col min="2" max="2" width="37.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="1"/>
     <col min="4" max="4" width="41.25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="35.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="23.375" style="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="1"/>
     <col min="8" max="8" width="25.25" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -664,185 +740,225 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="90">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="90">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="45">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="20.25" customHeight="1"/>
+    <row r="6" spans="1:9" ht="71.25">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="7"/>
-      <c r="H2" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="39.75" customHeight="1">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="20.25" customHeight="1"/>
-    <row r="6" spans="1:8" ht="42.75">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="85.5" customHeight="1">
+      <c r="H6" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="213.75">
       <c r="A7" s="2"/>
       <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1">
+        <v>21</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1">
+        <v>24</v>
+      </c>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" ht="42.75">
+        <v>25</v>
+      </c>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:9" ht="42.75">
       <c r="A10" s="2"/>
       <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:8" ht="15">
+        <v>26</v>
+      </c>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:9" ht="15">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1">
+    <row r="12" spans="1:9" ht="15" customHeight="1">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
-      <c r="D12" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="42.75">
+      <c r="D12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="11"/>
+    </row>
+    <row r="13" spans="1:9" ht="96.75" customHeight="1">
       <c r="A13" s="2"/>
       <c r="B13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" ht="48" customHeight="1">
+        <v>28</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:9" ht="57">
       <c r="A14" s="2"/>
       <c r="B14" s="3" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="45">
       <c r="A17" s="2" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H17" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="142.5">
+      <c r="A19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="60">
-      <c r="A19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="D19" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="8" t="s">
         <v>40</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="28.5">
       <c r="A20" s="2"/>
       <c r="B20" s="3" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="2"/>
       <c r="B21" s="3" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="150">
       <c r="A23" s="2" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="45">
+        <v>47</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="128.25">
       <c r="A25" s="2" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>42</v>
+        <v>52</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15">
       <c r="D27" s="4" t="s">
-        <v>43</v>
+        <v>55</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>